<commit_message>
Update charts to indicates Yoga
</commit_message>
<xml_diff>
--- a/docs_markdown/benchmark.xlsx
+++ b/docs_markdown/benchmark.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="989" activeTab="3"/>
+    <workbookView xWindow="40000" yWindow="-660" windowWidth="25600" windowHeight="16060" tabRatio="989" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="iPhone 7" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="iPhone 5" sheetId="4" r:id="rId4"/>
     <sheet name="Comparison" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1049,15 +1049,7 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:strRef>
-              <c:f>flexlayout</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>flexlayout</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>FlexLayout/Yoga</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28800">
@@ -1206,11 +1198,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2064664984"/>
-        <c:axId val="-2065440696"/>
+        <c:axId val="-2116475736"/>
+        <c:axId val="-2123233720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2064664984"/>
+        <c:axId val="-2116475736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1294,7 +1286,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2065440696"/>
+        <c:crossAx val="-2123233720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1302,7 +1294,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2065440696"/>
+        <c:axId val="-2123233720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1399,7 +1391,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2064664984"/>
+        <c:crossAx val="-2116475736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2225,11 +2217,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2056008776"/>
-        <c:axId val="-2055507256"/>
+        <c:axId val="-2114029672"/>
+        <c:axId val="-2060086280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2056008776"/>
+        <c:axId val="-2114029672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2313,7 +2305,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2055507256"/>
+        <c:crossAx val="-2060086280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2321,7 +2313,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2055507256"/>
+        <c:axId val="-2060086280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2380,7 +2372,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.00912179164569701"/>
+              <c:x val="0.009121791645697"/>
               <c:y val="0.395347883163768"/>
             </c:manualLayout>
           </c:layout>
@@ -2418,7 +2410,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2056008776"/>
+        <c:crossAx val="-2114029672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3231,15 +3223,7 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:strRef>
-              <c:f>flexlayout</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>flexlayout</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>FlexLayout/Yoga</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28800">
@@ -3388,11 +3372,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2055403784"/>
-        <c:axId val="-2055573960"/>
+        <c:axId val="-2059732104"/>
+        <c:axId val="-2059726024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2055403784"/>
+        <c:axId val="-2059732104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3476,7 +3460,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2055573960"/>
+        <c:crossAx val="-2059726024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3484,7 +3468,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2055573960"/>
+        <c:axId val="-2059726024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3581,7 +3565,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2055403784"/>
+        <c:crossAx val="-2059732104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4394,15 +4378,7 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:strRef>
-              <c:f>flexlayout</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>flexlayout</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>FlexLayout/Yoga</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28800">
@@ -4551,11 +4527,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2061390024"/>
-        <c:axId val="-2061383944"/>
+        <c:axId val="-2120010088"/>
+        <c:axId val="-2060990936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2061390024"/>
+        <c:axId val="-2120010088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4639,7 +4615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2061383944"/>
+        <c:crossAx val="-2060990936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4647,7 +4623,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2061383944"/>
+        <c:axId val="-2060990936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4744,7 +4720,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2061390024"/>
+        <c:crossAx val="-2120010088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5309,11 +5285,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2055482856"/>
-        <c:axId val="-2055476872"/>
+        <c:axId val="-2060891512"/>
+        <c:axId val="-2060885528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2055482856"/>
+        <c:axId val="-2060891512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5397,7 +5373,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2055476872"/>
+        <c:crossAx val="-2060885528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5405,7 +5381,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2055476872"/>
+        <c:axId val="-2060885528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5502,7 +5478,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2055482856"/>
+        <c:crossAx val="-2060891512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6057,7 +6033,7 @@
   <dimension ref="A52:L146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8823,7 +8799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A52:I130"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
@@ -13652,8 +13628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A52:I142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A142" sqref="A142"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>